<commit_message>
adicionado conexao ao banco do ECQ
</commit_message>
<xml_diff>
--- a/AHP-CRITERIOS_PESOS/AHP_consolidado.xlsx
+++ b/AHP-CRITERIOS_PESOS/AHP_consolidado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://timbrasil-my.sharepoint.com/personal/tblacerda_timbrasil_com_br/Documents/__Automacao_de_tarefas/HACK@TIM_2024/AHP-CRITERIOS_PESOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://timbrasil-my.sharepoint.com/personal/tblacerda_timbrasil_com_br/Documents/__Automacao_de_tarefas/HACK@TIM_2024/__ENTREGAVEIS_GRUPO_XX_DANTIMZIG__/PYTHON/AHP-CRITERIOS_PESOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_F25DC773A252ABDACC104865295C53F25ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA466705-3147-469B-B416-93F3EA5E788B}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_F25DC773A252ABDACC104865295C53F25ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA734018-4CE1-4F36-B197-3182CA8539F0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,17 +125,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,29 +142,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -209,16 +191,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -227,21 +208,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -609,10 +589,13 @@
   <dimension ref="A1:E235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E235" sqref="A1:E235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -627,41 +610,41 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B2" s="3">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="3">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -669,16 +652,16 @@
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B4" s="3">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -686,16 +669,16 @@
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>6</v>
       </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -703,16 +686,16 @@
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -720,16 +703,16 @@
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="3">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -737,16 +720,16 @@
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -754,16 +737,16 @@
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="4">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -771,16 +754,16 @@
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="4">
-        <v>3</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="3">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -788,16 +771,16 @@
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -805,16 +788,16 @@
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="4">
-        <v>7</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="B12" s="3">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -822,33 +805,33 @@
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="4">
-        <v>3</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="B13" s="3">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3">
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="2">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="A14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -856,16 +839,16 @@
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>2</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -873,16 +856,16 @@
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="4">
-        <v>3</v>
-      </c>
-      <c r="C16" s="4">
+      <c r="B16" s="3">
+        <v>3</v>
+      </c>
+      <c r="C16" s="3">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -890,16 +873,16 @@
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4">
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -907,16 +890,16 @@
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="4">
-        <v>3</v>
-      </c>
-      <c r="C18" s="4">
+      <c r="B18" s="3">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3">
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -924,16 +907,16 @@
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3">
         <v>3</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -941,16 +924,16 @@
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4">
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
         <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -958,16 +941,16 @@
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4">
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
         <v>3</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -975,16 +958,16 @@
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4">
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3">
         <v>5</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -992,16 +975,16 @@
       <c r="A23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="4">
-        <v>3</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="B23" s="3">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3">
         <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1009,16 +992,16 @@
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="4">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4">
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3">
         <v>3</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1026,16 +1009,16 @@
       <c r="A25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="4">
-        <v>3</v>
-      </c>
-      <c r="C25" s="4">
+      <c r="B25" s="3">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3">
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1049,10 +1032,10 @@
       <c r="C26" s="4">
         <v>1</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1066,10 +1049,10 @@
       <c r="C27" s="4">
         <v>1</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1083,10 +1066,10 @@
       <c r="C28" s="4">
         <v>1</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1100,10 +1083,10 @@
       <c r="C29" s="4">
         <v>5</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1117,10 +1100,10 @@
       <c r="C30" s="4">
         <v>3</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1134,10 +1117,10 @@
       <c r="C31" s="4">
         <v>7</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1151,10 +1134,10 @@
       <c r="C32" s="4">
         <v>9</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1168,10 +1151,10 @@
       <c r="C33" s="4">
         <v>3</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1185,10 +1168,10 @@
       <c r="C34" s="4">
         <v>3</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1202,10 +1185,10 @@
       <c r="C35" s="4">
         <v>1</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D35" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1219,10 +1202,10 @@
       <c r="C36" s="4">
         <v>5</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D36" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1236,10 +1219,10 @@
       <c r="C37" s="4">
         <v>1</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1253,10 +1236,10 @@
       <c r="C38" s="4">
         <v>5</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1270,10 +1253,10 @@
       <c r="C39" s="4">
         <v>3</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1287,10 +1270,10 @@
       <c r="C40" s="4">
         <v>7</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1304,10 +1287,10 @@
       <c r="C41" s="4">
         <v>9</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1321,10 +1304,10 @@
       <c r="C42" s="4">
         <v>1</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1338,10 +1321,10 @@
       <c r="C43" s="4">
         <v>3</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1355,10 +1338,10 @@
       <c r="C44" s="4">
         <v>3</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="D44" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1372,10 +1355,10 @@
       <c r="C45" s="4">
         <v>1</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1389,10 +1372,10 @@
       <c r="C46" s="4">
         <v>5</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1406,10 +1389,10 @@
       <c r="C47" s="4">
         <v>5</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1423,10 +1406,10 @@
       <c r="C48" s="4">
         <v>7</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1440,10 +1423,10 @@
       <c r="C49" s="4">
         <v>9</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1457,10 +1440,10 @@
       <c r="C50" s="4">
         <v>1</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1474,10 +1457,10 @@
       <c r="C51" s="4">
         <v>3</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1491,10 +1474,10 @@
       <c r="C52" s="4">
         <v>1</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1508,10 +1491,10 @@
       <c r="C53" s="4">
         <v>3</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1525,10 +1508,10 @@
       <c r="C54" s="4">
         <v>3</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1542,10 +1525,10 @@
       <c r="C55" s="4">
         <v>5</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1559,10 +1542,10 @@
       <c r="C56" s="4">
         <v>7</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1576,10 +1559,10 @@
       <c r="C57" s="4">
         <v>1</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1593,10 +1576,10 @@
       <c r="C58" s="4">
         <v>1</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1610,10 +1593,10 @@
       <c r="C59" s="4">
         <v>3</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1627,10 +1610,10 @@
       <c r="C60" s="4">
         <v>1</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1644,10 +1627,10 @@
       <c r="C61" s="4">
         <v>5</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1661,10 +1644,10 @@
       <c r="C62" s="4">
         <v>7</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1678,10 +1661,10 @@
       <c r="C63" s="4">
         <v>1</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1695,10 +1678,10 @@
       <c r="C64" s="4">
         <v>3</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1712,10 +1695,10 @@
       <c r="C65" s="4">
         <v>1</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1729,10 +1712,10 @@
       <c r="C66" s="4">
         <v>5</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1746,10 +1729,10 @@
       <c r="C67" s="4">
         <v>7</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1763,10 +1746,10 @@
       <c r="C68" s="4">
         <v>1</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1780,10 +1763,10 @@
       <c r="C69" s="4">
         <v>3</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1797,10 +1780,10 @@
       <c r="C70" s="4">
         <v>7</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1814,10 +1797,10 @@
       <c r="C71" s="4">
         <v>9</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1831,10 +1814,10 @@
       <c r="C72" s="4">
         <v>1</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1848,10 +1831,10 @@
       <c r="C73" s="4">
         <v>3</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D73" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1865,10 +1848,10 @@
       <c r="C74" s="4">
         <v>7</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D74" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1882,10 +1865,10 @@
       <c r="C75" s="4">
         <v>1</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D75" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1899,10 +1882,10 @@
       <c r="C76" s="4">
         <v>3</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D76" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1916,10 +1899,10 @@
       <c r="C77" s="4">
         <v>1</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D77" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1933,10 +1916,10 @@
       <c r="C78" s="4">
         <v>1</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D78" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1950,10 +1933,10 @@
       <c r="C79" s="4">
         <v>5</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D79" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1967,10 +1950,10 @@
       <c r="C80" s="4">
         <v>1</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E80" t="s">
+      <c r="D80" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E80" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1984,10 +1967,10 @@
       <c r="C81" s="4">
         <v>3</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D81" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2001,10 +1984,10 @@
       <c r="C82" s="4">
         <v>1</v>
       </c>
-      <c r="D82" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="D82" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E82" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2018,10 +2001,10 @@
       <c r="C83" s="4">
         <v>7</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E83" t="s">
+      <c r="D83" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2035,10 +2018,10 @@
       <c r="C84" s="4">
         <v>8</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" t="s">
+      <c r="D84" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2052,10 +2035,10 @@
       <c r="C85" s="4">
         <v>1</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2069,10 +2052,10 @@
       <c r="C86" s="4">
         <v>3</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D86" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2086,10 +2069,10 @@
       <c r="C87" s="4">
         <v>5</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D87" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2103,10 +2086,10 @@
       <c r="C88" s="4">
         <v>5</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="D88" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2120,10 +2103,10 @@
       <c r="C89" s="4">
         <v>9</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D89" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2137,10 +2120,10 @@
       <c r="C90" s="4">
         <v>3</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D90" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2154,10 +2137,10 @@
       <c r="C91" s="4">
         <v>3</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D91" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2171,10 +2154,10 @@
       <c r="C92" s="4">
         <v>1</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D92" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2188,10 +2171,10 @@
       <c r="C93" s="4">
         <v>3</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E93" t="s">
+      <c r="D93" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2205,10 +2188,10 @@
       <c r="C94" s="4">
         <v>7</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E94" t="s">
+      <c r="D94" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2222,10 +2205,10 @@
       <c r="C95" s="4">
         <v>8</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E95" t="s">
+      <c r="D95" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2239,10 +2222,10 @@
       <c r="C96" s="4">
         <v>1</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D96" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2256,10 +2239,10 @@
       <c r="C97" s="4">
         <v>1</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="D97" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2273,10 +2256,10 @@
       <c r="C98" s="4">
         <v>1</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D98" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2290,10 +2273,10 @@
       <c r="C99" s="4">
         <v>1</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D99" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2307,10 +2290,10 @@
       <c r="C100" s="4">
         <v>9</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D100" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2324,10 +2307,10 @@
       <c r="C101" s="4">
         <v>1</v>
       </c>
-      <c r="D101" s="3" t="s">
+      <c r="D101" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2341,10 +2324,10 @@
       <c r="C102" s="4">
         <v>1</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="D102" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2358,10 +2341,10 @@
       <c r="C103" s="4">
         <v>2</v>
       </c>
-      <c r="D103" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E103" t="s">
+      <c r="D103" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E103" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2375,10 +2358,10 @@
       <c r="C104" s="4">
         <v>7</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="D104" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E104" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2392,10 +2375,10 @@
       <c r="C105" s="4">
         <v>9</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E105" t="s">
+      <c r="D105" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2409,10 +2392,10 @@
       <c r="C106" s="4">
         <v>1</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="D106" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E106" t="s">
+      <c r="E106" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2426,10 +2409,10 @@
       <c r="C107" s="4">
         <v>1</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="D107" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E107" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2443,10 +2426,10 @@
       <c r="C108" s="4">
         <v>5</v>
       </c>
-      <c r="D108" s="3" t="s">
+      <c r="D108" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2460,10 +2443,10 @@
       <c r="C109" s="4">
         <v>5</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="D109" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E109" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2477,10 +2460,10 @@
       <c r="C110" s="4">
         <v>9</v>
       </c>
-      <c r="D110" s="3" t="s">
+      <c r="D110" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E110" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2494,10 +2477,10 @@
       <c r="C111" s="4">
         <v>3</v>
       </c>
-      <c r="D111" s="3" t="s">
+      <c r="D111" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2511,10 +2494,10 @@
       <c r="C112" s="4">
         <v>3</v>
       </c>
-      <c r="D112" s="3" t="s">
+      <c r="D112" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E112" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2528,10 +2511,10 @@
       <c r="C113" s="4">
         <v>7</v>
       </c>
-      <c r="D113" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E113" t="s">
+      <c r="D113" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E113" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2545,10 +2528,10 @@
       <c r="C114" s="4">
         <v>8</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E114" t="s">
+      <c r="D114" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2562,10 +2545,10 @@
       <c r="C115" s="4">
         <v>8</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D115" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E115" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2579,10 +2562,10 @@
       <c r="C116" s="4">
         <v>1</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="D116" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2596,10 +2579,10 @@
       <c r="C117" s="4">
         <v>1</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D117" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E117" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2613,10 +2596,10 @@
       <c r="C118" s="4">
         <v>1</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D118" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E118" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2630,10 +2613,10 @@
       <c r="C119" s="4">
         <v>1</v>
       </c>
-      <c r="D119" s="3" t="s">
+      <c r="D119" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E119" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2647,10 +2630,10 @@
       <c r="C120" s="4">
         <v>1</v>
       </c>
-      <c r="D120" s="3" t="s">
+      <c r="D120" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E120" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2664,10 +2647,10 @@
       <c r="C121" s="4">
         <v>1</v>
       </c>
-      <c r="D121" s="3" t="s">
+      <c r="D121" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E121" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2681,10 +2664,10 @@
       <c r="C122" s="4">
         <v>3</v>
       </c>
-      <c r="D122" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E122" t="s">
+      <c r="D122" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2698,10 +2681,10 @@
       <c r="C123" s="4">
         <v>3</v>
       </c>
-      <c r="D123" s="3" t="s">
+      <c r="D123" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E123" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2715,10 +2698,10 @@
       <c r="C124" s="4">
         <v>3</v>
       </c>
-      <c r="D124" s="3" t="s">
+      <c r="D124" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E124" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2732,10 +2715,10 @@
       <c r="C125" s="4">
         <v>3</v>
       </c>
-      <c r="D125" s="3" t="s">
+      <c r="D125" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E125" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2749,10 +2732,10 @@
       <c r="C126" s="4">
         <v>3</v>
       </c>
-      <c r="D126" s="3" t="s">
+      <c r="D126" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E126" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2766,10 +2749,10 @@
       <c r="C127" s="4">
         <v>3</v>
       </c>
-      <c r="D127" s="3" t="s">
+      <c r="D127" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E127" t="s">
+      <c r="E127" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2783,10 +2766,10 @@
       <c r="C128" s="4">
         <v>3</v>
       </c>
-      <c r="D128" s="3" t="s">
+      <c r="D128" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E128" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2800,10 +2783,10 @@
       <c r="C129" s="4">
         <v>3</v>
       </c>
-      <c r="D129" s="3" t="s">
+      <c r="D129" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E129" t="s">
+      <c r="E129" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2817,10 +2800,10 @@
       <c r="C130" s="4">
         <v>2</v>
       </c>
-      <c r="D130" s="3" t="s">
+      <c r="D130" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E130" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2834,10 +2817,10 @@
       <c r="C131" s="4">
         <v>2</v>
       </c>
-      <c r="D131" s="3" t="s">
+      <c r="D131" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E131" t="s">
+      <c r="E131" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2851,10 +2834,10 @@
       <c r="C132" s="4">
         <v>2</v>
       </c>
-      <c r="D132" s="3" t="s">
+      <c r="D132" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E132" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2868,10 +2851,10 @@
       <c r="C133" s="4">
         <v>2</v>
       </c>
-      <c r="D133" s="3" t="s">
+      <c r="D133" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E133" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2885,10 +2868,10 @@
       <c r="C134" s="4">
         <v>9</v>
       </c>
-      <c r="D134" s="3" t="s">
+      <c r="D134" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E134" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2902,10 +2885,10 @@
       <c r="C135" s="4">
         <v>2</v>
       </c>
-      <c r="D135" s="3" t="s">
+      <c r="D135" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E135" t="s">
+      <c r="E135" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2919,10 +2902,10 @@
       <c r="C136" s="4">
         <v>2</v>
       </c>
-      <c r="D136" s="3" t="s">
+      <c r="D136" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E136" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2936,10 +2919,10 @@
       <c r="C137" s="4">
         <v>8</v>
       </c>
-      <c r="D137" s="3" t="s">
+      <c r="D137" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E137" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2953,10 +2936,10 @@
       <c r="C138" s="4">
         <v>7</v>
       </c>
-      <c r="D138" s="3" t="s">
+      <c r="D138" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E138" t="s">
+      <c r="E138" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2970,10 +2953,10 @@
       <c r="C139" s="4">
         <v>1</v>
       </c>
-      <c r="D139" s="3" t="s">
+      <c r="D139" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E139" t="s">
+      <c r="E139" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2987,10 +2970,10 @@
       <c r="C140" s="4">
         <v>9</v>
       </c>
-      <c r="D140" s="3" t="s">
+      <c r="D140" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E140" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3004,10 +2987,10 @@
       <c r="C141" s="4">
         <v>1</v>
       </c>
-      <c r="D141" s="3" t="s">
+      <c r="D141" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E141" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3021,10 +3004,10 @@
       <c r="C142" s="4">
         <v>1</v>
       </c>
-      <c r="D142" s="3" t="s">
+      <c r="D142" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E142" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3038,10 +3021,10 @@
       <c r="C143" s="4">
         <v>8</v>
       </c>
-      <c r="D143" s="3" t="s">
+      <c r="D143" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E143" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3055,10 +3038,10 @@
       <c r="C144" s="4">
         <v>7</v>
       </c>
-      <c r="D144" s="3" t="s">
+      <c r="D144" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E144" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3072,10 +3055,10 @@
       <c r="C145" s="4">
         <v>9</v>
       </c>
-      <c r="D145" s="3" t="s">
+      <c r="D145" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E145" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3089,10 +3072,10 @@
       <c r="C146" s="4">
         <v>1</v>
       </c>
-      <c r="D146" s="3" t="s">
+      <c r="D146" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E146" t="s">
+      <c r="E146" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3106,10 +3089,10 @@
       <c r="C147" s="4">
         <v>1</v>
       </c>
-      <c r="D147" s="3" t="s">
+      <c r="D147" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E147" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3123,10 +3106,10 @@
       <c r="C148" s="4">
         <v>1</v>
       </c>
-      <c r="D148" s="3" t="s">
+      <c r="D148" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E148" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3140,10 +3123,10 @@
       <c r="C149" s="4">
         <v>9</v>
       </c>
-      <c r="D149" s="3" t="s">
+      <c r="D149" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E149" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3157,10 +3140,10 @@
       <c r="C150" s="4">
         <v>1</v>
       </c>
-      <c r="D150" s="3" t="s">
+      <c r="D150" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E150" t="s">
+      <c r="E150" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3174,10 +3157,10 @@
       <c r="C151" s="4">
         <v>1</v>
       </c>
-      <c r="D151" s="3" t="s">
+      <c r="D151" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E151" t="s">
+      <c r="E151" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3191,10 +3174,10 @@
       <c r="C152" s="4">
         <v>9</v>
       </c>
-      <c r="D152" s="3" t="s">
+      <c r="D152" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E152" t="s">
+      <c r="E152" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3208,10 +3191,10 @@
       <c r="C153" s="4">
         <v>2</v>
       </c>
-      <c r="D153" s="3" t="s">
+      <c r="D153" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E153" t="s">
+      <c r="E153" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3225,10 +3208,10 @@
       <c r="C154" s="4">
         <v>1</v>
       </c>
-      <c r="D154" s="3" t="s">
+      <c r="D154" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E154" t="s">
+      <c r="E154" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3242,10 +3225,10 @@
       <c r="C155" s="4">
         <v>3</v>
       </c>
-      <c r="D155" s="3" t="s">
+      <c r="D155" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E155" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3259,10 +3242,10 @@
       <c r="C156" s="4">
         <v>3</v>
       </c>
-      <c r="D156" s="3" t="s">
+      <c r="D156" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E156" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3276,1336 +3259,1336 @@
       <c r="C157" s="4">
         <v>3</v>
       </c>
-      <c r="D157" s="3" t="s">
+      <c r="D157" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E157" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" s="7" t="s">
+      <c r="A158" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B158" s="8">
-        <v>5</v>
-      </c>
-      <c r="C158" s="8">
-        <v>1</v>
-      </c>
-      <c r="D158" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E158" t="s">
+      <c r="B158" s="7">
+        <v>5</v>
+      </c>
+      <c r="C158" s="7">
+        <v>1</v>
+      </c>
+      <c r="D158" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E158" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" s="7" t="s">
+      <c r="A159" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B159" s="8">
-        <v>5</v>
-      </c>
-      <c r="C159" s="8">
-        <v>1</v>
-      </c>
-      <c r="D159" s="7" t="s">
+      <c r="B159" s="7">
+        <v>5</v>
+      </c>
+      <c r="C159" s="7">
+        <v>1</v>
+      </c>
+      <c r="D159" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E159" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="7" t="s">
+      <c r="A160" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B160" s="8">
-        <v>7</v>
-      </c>
-      <c r="C160" s="8">
-        <v>1</v>
-      </c>
-      <c r="D160" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E160" t="s">
+      <c r="B160" s="7">
+        <v>7</v>
+      </c>
+      <c r="C160" s="7">
+        <v>1</v>
+      </c>
+      <c r="D160" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E160" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" s="7" t="s">
+      <c r="A161" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B161" s="8">
-        <v>7</v>
-      </c>
-      <c r="C161" s="8">
-        <v>1</v>
-      </c>
-      <c r="D161" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E161" t="s">
+      <c r="B161" s="7">
+        <v>7</v>
+      </c>
+      <c r="C161" s="7">
+        <v>1</v>
+      </c>
+      <c r="D161" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E161" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="7" t="s">
+      <c r="A162" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B162" s="8">
-        <v>7</v>
-      </c>
-      <c r="C162" s="8">
-        <v>1</v>
-      </c>
-      <c r="D162" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E162" t="s">
+      <c r="B162" s="7">
+        <v>7</v>
+      </c>
+      <c r="C162" s="7">
+        <v>1</v>
+      </c>
+      <c r="D162" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E162" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" s="7" t="s">
+      <c r="A163" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B163" s="8">
-        <v>7</v>
-      </c>
-      <c r="C163" s="8">
-        <v>1</v>
-      </c>
-      <c r="D163" s="7" t="s">
+      <c r="B163" s="7">
+        <v>7</v>
+      </c>
+      <c r="C163" s="7">
+        <v>1</v>
+      </c>
+      <c r="D163" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E163" t="s">
+      <c r="E163" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" s="7" t="s">
+      <c r="A164" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B164" s="8">
-        <v>8</v>
-      </c>
-      <c r="C164" s="8">
-        <v>1</v>
-      </c>
-      <c r="D164" s="7" t="s">
+      <c r="B164" s="7">
+        <v>8</v>
+      </c>
+      <c r="C164" s="7">
+        <v>1</v>
+      </c>
+      <c r="D164" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E164" t="s">
+      <c r="E164" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="7" t="s">
+      <c r="A165" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B165" s="8">
+      <c r="B165" s="7">
         <v>4</v>
       </c>
-      <c r="C165" s="8">
-        <v>1</v>
-      </c>
-      <c r="D165" s="7" t="s">
+      <c r="C165" s="7">
+        <v>1</v>
+      </c>
+      <c r="D165" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="7" t="s">
+      <c r="A166" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B166" s="8">
+      <c r="B166" s="7">
         <v>4</v>
       </c>
-      <c r="C166" s="8">
-        <v>1</v>
-      </c>
-      <c r="D166" s="7" t="s">
+      <c r="C166" s="7">
+        <v>1</v>
+      </c>
+      <c r="D166" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="7" t="s">
+      <c r="A167" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B167" s="8">
-        <v>3</v>
-      </c>
-      <c r="C167" s="8">
-        <v>1</v>
-      </c>
-      <c r="D167" s="7" t="s">
+      <c r="B167" s="7">
+        <v>3</v>
+      </c>
+      <c r="C167" s="7">
+        <v>1</v>
+      </c>
+      <c r="D167" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" s="7" t="s">
+      <c r="A168" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B168" s="8">
-        <v>9</v>
-      </c>
-      <c r="C168" s="8">
-        <v>1</v>
-      </c>
-      <c r="D168" s="7" t="s">
+      <c r="B168" s="7">
+        <v>9</v>
+      </c>
+      <c r="C168" s="7">
+        <v>1</v>
+      </c>
+      <c r="D168" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E168" t="s">
+      <c r="E168" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" s="7" t="s">
+      <c r="A169" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B169" s="8">
+      <c r="B169" s="7">
         <v>4</v>
       </c>
-      <c r="C169" s="8">
-        <v>1</v>
-      </c>
-      <c r="D169" s="7" t="s">
+      <c r="C169" s="7">
+        <v>1</v>
+      </c>
+      <c r="D169" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B170" s="8">
-        <v>1</v>
-      </c>
-      <c r="C170" s="8">
+      <c r="A170" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B170" s="7">
+        <v>1</v>
+      </c>
+      <c r="C170" s="7">
         <v>2</v>
       </c>
-      <c r="D170" s="7" t="s">
+      <c r="D170" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B171" s="8">
-        <v>5</v>
-      </c>
-      <c r="C171" s="8">
-        <v>1</v>
-      </c>
-      <c r="D171" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E171" t="s">
+      <c r="A171" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B171" s="7">
+        <v>5</v>
+      </c>
+      <c r="C171" s="7">
+        <v>1</v>
+      </c>
+      <c r="D171" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E171" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B172" s="8">
-        <v>5</v>
-      </c>
-      <c r="C172" s="8">
-        <v>1</v>
-      </c>
-      <c r="D172" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E172" t="s">
+      <c r="A172" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B172" s="7">
+        <v>5</v>
+      </c>
+      <c r="C172" s="7">
+        <v>1</v>
+      </c>
+      <c r="D172" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E172" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B173" s="8">
-        <v>5</v>
-      </c>
-      <c r="C173" s="8">
-        <v>1</v>
-      </c>
-      <c r="D173" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E173" t="s">
+      <c r="A173" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B173" s="7">
+        <v>5</v>
+      </c>
+      <c r="C173" s="7">
+        <v>1</v>
+      </c>
+      <c r="D173" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E173" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B174" s="8">
-        <v>5</v>
-      </c>
-      <c r="C174" s="8">
-        <v>1</v>
-      </c>
-      <c r="D174" s="7" t="s">
+      <c r="A174" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B174" s="7">
+        <v>5</v>
+      </c>
+      <c r="C174" s="7">
+        <v>1</v>
+      </c>
+      <c r="D174" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E174" t="s">
+      <c r="E174" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B175" s="8">
-        <v>9</v>
-      </c>
-      <c r="C175" s="8">
-        <v>1</v>
-      </c>
-      <c r="D175" s="7" t="s">
+      <c r="A175" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B175" s="7">
+        <v>9</v>
+      </c>
+      <c r="C175" s="7">
+        <v>1</v>
+      </c>
+      <c r="D175" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E175" t="s">
+      <c r="E175" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B176" s="8">
-        <v>1</v>
-      </c>
-      <c r="C176" s="8">
+      <c r="A176" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B176" s="7">
+        <v>1</v>
+      </c>
+      <c r="C176" s="7">
         <v>4</v>
       </c>
-      <c r="D176" s="7" t="s">
+      <c r="D176" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E176" t="s">
+      <c r="E176" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B177" s="8">
-        <v>1</v>
-      </c>
-      <c r="C177" s="8">
-        <v>5</v>
-      </c>
-      <c r="D177" s="7" t="s">
+      <c r="A177" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B177" s="7">
+        <v>1</v>
+      </c>
+      <c r="C177" s="7">
+        <v>5</v>
+      </c>
+      <c r="D177" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B178" s="8">
-        <v>1</v>
-      </c>
-      <c r="C178" s="8">
-        <v>9</v>
-      </c>
-      <c r="D178" s="7" t="s">
+      <c r="A178" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B178" s="7">
+        <v>1</v>
+      </c>
+      <c r="C178" s="7">
+        <v>9</v>
+      </c>
+      <c r="D178" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B179" s="8">
-        <v>9</v>
-      </c>
-      <c r="C179" s="8">
-        <v>1</v>
-      </c>
-      <c r="D179" s="7" t="s">
+      <c r="A179" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B179" s="7">
+        <v>9</v>
+      </c>
+      <c r="C179" s="7">
+        <v>1</v>
+      </c>
+      <c r="D179" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B180" s="8">
-        <v>3</v>
-      </c>
-      <c r="C180" s="8">
-        <v>1</v>
-      </c>
-      <c r="D180" s="7" t="s">
+      <c r="A180" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B180" s="7">
+        <v>3</v>
+      </c>
+      <c r="C180" s="7">
+        <v>1</v>
+      </c>
+      <c r="D180" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A181" s="7" t="s">
+      <c r="A181" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B181" s="8">
-        <v>5</v>
-      </c>
-      <c r="C181" s="8">
-        <v>1</v>
-      </c>
-      <c r="D181" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E181" t="s">
+      <c r="B181" s="7">
+        <v>5</v>
+      </c>
+      <c r="C181" s="7">
+        <v>1</v>
+      </c>
+      <c r="D181" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E181" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" s="7" t="s">
+      <c r="A182" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B182" s="8">
-        <v>5</v>
-      </c>
-      <c r="C182" s="8">
-        <v>1</v>
-      </c>
-      <c r="D182" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E182" t="s">
+      <c r="B182" s="7">
+        <v>5</v>
+      </c>
+      <c r="C182" s="7">
+        <v>1</v>
+      </c>
+      <c r="D182" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E182" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="7" t="s">
+      <c r="A183" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B183" s="8">
-        <v>5</v>
-      </c>
-      <c r="C183" s="8">
-        <v>1</v>
-      </c>
-      <c r="D183" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E183" t="s">
+      <c r="B183" s="7">
+        <v>5</v>
+      </c>
+      <c r="C183" s="7">
+        <v>1</v>
+      </c>
+      <c r="D183" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E183" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" s="7" t="s">
+      <c r="A184" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B184" s="8">
-        <v>5</v>
-      </c>
-      <c r="C184" s="8">
-        <v>1</v>
-      </c>
-      <c r="D184" s="7" t="s">
+      <c r="B184" s="7">
+        <v>5</v>
+      </c>
+      <c r="C184" s="7">
+        <v>1</v>
+      </c>
+      <c r="D184" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" s="7" t="s">
+      <c r="A185" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B185" s="8">
-        <v>9</v>
-      </c>
-      <c r="C185" s="8">
-        <v>1</v>
-      </c>
-      <c r="D185" s="7" t="s">
+      <c r="B185" s="7">
+        <v>9</v>
+      </c>
+      <c r="C185" s="7">
+        <v>1</v>
+      </c>
+      <c r="D185" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" s="7" t="s">
+      <c r="A186" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B186" s="8">
-        <v>1</v>
-      </c>
-      <c r="C186" s="8">
+      <c r="B186" s="7">
+        <v>1</v>
+      </c>
+      <c r="C186" s="7">
         <v>4</v>
       </c>
-      <c r="D186" s="7" t="s">
+      <c r="D186" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E186" t="s">
+      <c r="E186" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" s="7" t="s">
+      <c r="A187" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B187" s="8">
-        <v>1</v>
-      </c>
-      <c r="C187" s="8">
-        <v>5</v>
-      </c>
-      <c r="D187" s="7" t="s">
+      <c r="B187" s="7">
+        <v>1</v>
+      </c>
+      <c r="C187" s="7">
+        <v>5</v>
+      </c>
+      <c r="D187" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="7" t="s">
+      <c r="A188" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B188" s="8">
-        <v>1</v>
-      </c>
-      <c r="C188" s="8">
-        <v>9</v>
-      </c>
-      <c r="D188" s="7" t="s">
+      <c r="B188" s="7">
+        <v>1</v>
+      </c>
+      <c r="C188" s="7">
+        <v>9</v>
+      </c>
+      <c r="D188" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" s="7" t="s">
+      <c r="A189" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B189" s="8">
-        <v>9</v>
-      </c>
-      <c r="C189" s="8">
-        <v>1</v>
-      </c>
-      <c r="D189" s="7" t="s">
+      <c r="B189" s="7">
+        <v>9</v>
+      </c>
+      <c r="C189" s="7">
+        <v>1</v>
+      </c>
+      <c r="D189" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E189" t="s">
+      <c r="E189" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" s="7" t="s">
+      <c r="A190" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B190" s="8">
+      <c r="B190" s="7">
         <v>4</v>
       </c>
-      <c r="C190" s="8">
-        <v>1</v>
-      </c>
-      <c r="D190" s="7" t="s">
+      <c r="C190" s="7">
+        <v>1</v>
+      </c>
+      <c r="D190" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B191" s="8">
-        <v>1</v>
-      </c>
-      <c r="C191" s="8">
-        <v>1</v>
-      </c>
-      <c r="D191" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E191" t="s">
+      <c r="A191" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B191" s="7">
+        <v>1</v>
+      </c>
+      <c r="C191" s="7">
+        <v>1</v>
+      </c>
+      <c r="D191" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E191" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B192" s="8">
-        <v>1</v>
-      </c>
-      <c r="C192" s="8">
+      <c r="A192" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B192" s="7">
+        <v>1</v>
+      </c>
+      <c r="C192" s="7">
         <v>2</v>
       </c>
-      <c r="D192" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E192" t="s">
+      <c r="D192" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E192" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A193" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B193" s="8">
-        <v>1</v>
-      </c>
-      <c r="C193" s="8">
-        <v>1</v>
-      </c>
-      <c r="D193" s="7" t="s">
+      <c r="A193" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B193" s="7">
+        <v>1</v>
+      </c>
+      <c r="C193" s="7">
+        <v>1</v>
+      </c>
+      <c r="D193" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E193" t="s">
+      <c r="E193" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A194" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B194" s="8">
-        <v>1</v>
-      </c>
-      <c r="C194" s="8">
+      <c r="A194" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B194" s="7">
+        <v>1</v>
+      </c>
+      <c r="C194" s="7">
         <v>2</v>
       </c>
-      <c r="D194" s="7" t="s">
+      <c r="D194" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E194" t="s">
+      <c r="E194" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A195" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B195" s="8">
-        <v>1</v>
-      </c>
-      <c r="C195" s="8">
-        <v>5</v>
-      </c>
-      <c r="D195" s="7" t="s">
+      <c r="A195" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B195" s="7">
+        <v>1</v>
+      </c>
+      <c r="C195" s="7">
+        <v>5</v>
+      </c>
+      <c r="D195" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A196" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B196" s="8">
-        <v>1</v>
-      </c>
-      <c r="C196" s="8">
-        <v>5</v>
-      </c>
-      <c r="D196" s="7" t="s">
+      <c r="A196" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B196" s="7">
+        <v>1</v>
+      </c>
+      <c r="C196" s="7">
+        <v>5</v>
+      </c>
+      <c r="D196" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B197" s="8">
-        <v>1</v>
-      </c>
-      <c r="C197" s="8">
-        <v>8</v>
-      </c>
-      <c r="D197" s="7" t="s">
+      <c r="A197" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B197" s="7">
+        <v>1</v>
+      </c>
+      <c r="C197" s="7">
+        <v>8</v>
+      </c>
+      <c r="D197" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E197" t="s">
+      <c r="E197" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B198" s="8">
-        <v>1</v>
-      </c>
-      <c r="C198" s="8">
-        <v>1</v>
-      </c>
-      <c r="D198" s="7" t="s">
+      <c r="A198" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B198" s="7">
+        <v>1</v>
+      </c>
+      <c r="C198" s="7">
+        <v>1</v>
+      </c>
+      <c r="D198" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E198" t="s">
+      <c r="E198" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B199" s="8">
-        <v>1</v>
-      </c>
-      <c r="C199" s="8">
+      <c r="A199" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B199" s="7">
+        <v>1</v>
+      </c>
+      <c r="C199" s="7">
         <v>2</v>
       </c>
-      <c r="D199" s="7" t="s">
+      <c r="D199" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E199" t="s">
+      <c r="E199" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B200" s="8">
-        <v>1</v>
-      </c>
-      <c r="C200" s="8">
-        <v>1</v>
-      </c>
-      <c r="D200" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E200" t="s">
+      <c r="A200" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B200" s="7">
+        <v>1</v>
+      </c>
+      <c r="C200" s="7">
+        <v>1</v>
+      </c>
+      <c r="D200" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E200" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B201" s="8">
-        <v>1</v>
-      </c>
-      <c r="C201" s="8">
-        <v>1</v>
-      </c>
-      <c r="D201" s="7" t="s">
+      <c r="A201" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B201" s="7">
+        <v>1</v>
+      </c>
+      <c r="C201" s="7">
+        <v>1</v>
+      </c>
+      <c r="D201" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E201" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A202" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B202" s="8">
-        <v>1</v>
-      </c>
-      <c r="C202" s="8">
+      <c r="A202" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B202" s="7">
+        <v>1</v>
+      </c>
+      <c r="C202" s="7">
         <v>4</v>
       </c>
-      <c r="D202" s="7" t="s">
+      <c r="D202" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E202" t="s">
+      <c r="E202" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A203" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B203" s="8">
-        <v>1</v>
-      </c>
-      <c r="C203" s="8">
+      <c r="A203" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B203" s="7">
+        <v>1</v>
+      </c>
+      <c r="C203" s="7">
         <v>4</v>
       </c>
-      <c r="D203" s="7" t="s">
+      <c r="D203" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E203" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A204" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B204" s="8">
-        <v>1</v>
-      </c>
-      <c r="C204" s="8">
-        <v>5</v>
-      </c>
-      <c r="D204" s="7" t="s">
+      <c r="A204" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B204" s="7">
+        <v>1</v>
+      </c>
+      <c r="C204" s="7">
+        <v>5</v>
+      </c>
+      <c r="D204" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E204" t="s">
+      <c r="E204" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B205" s="8">
-        <v>1</v>
-      </c>
-      <c r="C205" s="8">
-        <v>9</v>
-      </c>
-      <c r="D205" s="7" t="s">
+      <c r="A205" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B205" s="7">
+        <v>1</v>
+      </c>
+      <c r="C205" s="7">
+        <v>9</v>
+      </c>
+      <c r="D205" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E205" t="s">
+      <c r="E205" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B206" s="8">
-        <v>1</v>
-      </c>
-      <c r="C206" s="8">
-        <v>1</v>
-      </c>
-      <c r="D206" s="7" t="s">
+      <c r="A206" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B206" s="7">
+        <v>1</v>
+      </c>
+      <c r="C206" s="7">
+        <v>1</v>
+      </c>
+      <c r="D206" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E206" t="s">
+      <c r="E206" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A207" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B207" s="8">
-        <v>1</v>
-      </c>
-      <c r="C207" s="8">
+      <c r="A207" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B207" s="7">
+        <v>1</v>
+      </c>
+      <c r="C207" s="7">
         <v>2</v>
       </c>
-      <c r="D207" s="7" t="s">
+      <c r="D207" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E207" t="s">
+      <c r="E207" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A208" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B208" s="8">
-        <v>3</v>
-      </c>
-      <c r="C208" s="8">
-        <v>1</v>
-      </c>
-      <c r="D208" s="7" t="s">
+      <c r="A208" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B208" s="7">
+        <v>3</v>
+      </c>
+      <c r="C208" s="7">
+        <v>1</v>
+      </c>
+      <c r="D208" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E208" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A209" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B209" s="8">
+      <c r="A209" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B209" s="7">
         <v>2</v>
       </c>
-      <c r="C209" s="8">
-        <v>1</v>
-      </c>
-      <c r="D209" s="7" t="s">
+      <c r="C209" s="7">
+        <v>1</v>
+      </c>
+      <c r="D209" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E209" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A210" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B210" s="8">
-        <v>1</v>
-      </c>
-      <c r="C210" s="8">
-        <v>3</v>
-      </c>
-      <c r="D210" s="7" t="s">
+      <c r="A210" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B210" s="7">
+        <v>1</v>
+      </c>
+      <c r="C210" s="7">
+        <v>3</v>
+      </c>
+      <c r="D210" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A211" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B211" s="8">
-        <v>1</v>
-      </c>
-      <c r="C211" s="8">
-        <v>3</v>
-      </c>
-      <c r="D211" s="7" t="s">
+      <c r="A211" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B211" s="7">
+        <v>1</v>
+      </c>
+      <c r="C211" s="7">
+        <v>3</v>
+      </c>
+      <c r="D211" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E211" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A212" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B212" s="8">
-        <v>1</v>
-      </c>
-      <c r="C212" s="8">
-        <v>7</v>
-      </c>
-      <c r="D212" s="7" t="s">
+      <c r="A212" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B212" s="7">
+        <v>1</v>
+      </c>
+      <c r="C212" s="7">
+        <v>7</v>
+      </c>
+      <c r="D212" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E212" t="s">
+      <c r="E212" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A213" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B213" s="8">
-        <v>1</v>
-      </c>
-      <c r="C213" s="8">
-        <v>1</v>
-      </c>
-      <c r="D213" s="7" t="s">
+      <c r="A213" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B213" s="7">
+        <v>1</v>
+      </c>
+      <c r="C213" s="7">
+        <v>1</v>
+      </c>
+      <c r="D213" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E213" t="s">
+      <c r="E213" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A214" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B214" s="8">
-        <v>1</v>
-      </c>
-      <c r="C214" s="8">
+      <c r="A214" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B214" s="7">
+        <v>1</v>
+      </c>
+      <c r="C214" s="7">
         <v>2</v>
       </c>
-      <c r="D214" s="7" t="s">
+      <c r="D214" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E214" t="s">
+      <c r="E214" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A215" s="7" t="s">
+      <c r="A215" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B215" s="8">
-        <v>1</v>
-      </c>
-      <c r="C215" s="8">
+      <c r="B215" s="7">
+        <v>1</v>
+      </c>
+      <c r="C215" s="7">
         <v>4</v>
       </c>
-      <c r="D215" s="7" t="s">
+      <c r="D215" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A216" s="7" t="s">
+      <c r="A216" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B216" s="8">
-        <v>1</v>
-      </c>
-      <c r="C216" s="8">
+      <c r="B216" s="7">
+        <v>1</v>
+      </c>
+      <c r="C216" s="7">
         <v>4</v>
       </c>
-      <c r="D216" s="7" t="s">
+      <c r="D216" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E216" t="s">
+      <c r="E216" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A217" s="7" t="s">
+      <c r="A217" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B217" s="8">
-        <v>1</v>
-      </c>
-      <c r="C217" s="8">
-        <v>5</v>
-      </c>
-      <c r="D217" s="7" t="s">
+      <c r="B217" s="7">
+        <v>1</v>
+      </c>
+      <c r="C217" s="7">
+        <v>5</v>
+      </c>
+      <c r="D217" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E217" t="s">
+      <c r="E217" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A218" s="7" t="s">
+      <c r="A218" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B218" s="8">
-        <v>1</v>
-      </c>
-      <c r="C218" s="8">
-        <v>9</v>
-      </c>
-      <c r="D218" s="7" t="s">
+      <c r="B218" s="7">
+        <v>1</v>
+      </c>
+      <c r="C218" s="7">
+        <v>9</v>
+      </c>
+      <c r="D218" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E218" t="s">
+      <c r="E218" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A219" s="7" t="s">
+      <c r="A219" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B219" s="8">
-        <v>1</v>
-      </c>
-      <c r="C219" s="8">
-        <v>1</v>
-      </c>
-      <c r="D219" s="7" t="s">
+      <c r="B219" s="7">
+        <v>1</v>
+      </c>
+      <c r="C219" s="7">
+        <v>1</v>
+      </c>
+      <c r="D219" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E219" t="s">
+      <c r="E219" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A220" s="7" t="s">
+      <c r="A220" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B220" s="8">
-        <v>1</v>
-      </c>
-      <c r="C220" s="8">
+      <c r="B220" s="7">
+        <v>1</v>
+      </c>
+      <c r="C220" s="7">
         <v>2</v>
       </c>
-      <c r="D220" s="7" t="s">
+      <c r="D220" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E220" t="s">
+      <c r="E220" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A221" s="7" t="s">
+      <c r="A221" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B221" s="8">
-        <v>1</v>
-      </c>
-      <c r="C221" s="8">
-        <v>9</v>
-      </c>
-      <c r="D221" s="7" t="s">
+      <c r="B221" s="7">
+        <v>1</v>
+      </c>
+      <c r="C221" s="7">
+        <v>9</v>
+      </c>
+      <c r="D221" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E221" t="s">
+      <c r="E221" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A222" s="7" t="s">
+      <c r="A222" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B222" s="8">
-        <v>1</v>
-      </c>
-      <c r="C222" s="8">
-        <v>9</v>
-      </c>
-      <c r="D222" s="7" t="s">
+      <c r="B222" s="7">
+        <v>1</v>
+      </c>
+      <c r="C222" s="7">
+        <v>9</v>
+      </c>
+      <c r="D222" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E222" t="s">
+      <c r="E222" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A223" s="7" t="s">
+      <c r="A223" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B223" s="8">
-        <v>1</v>
-      </c>
-      <c r="C223" s="8">
-        <v>9</v>
-      </c>
-      <c r="D223" s="7" t="s">
+      <c r="B223" s="7">
+        <v>1</v>
+      </c>
+      <c r="C223" s="7">
+        <v>9</v>
+      </c>
+      <c r="D223" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E223" t="s">
+      <c r="E223" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A224" s="7" t="s">
+      <c r="A224" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B224" s="8">
-        <v>1</v>
-      </c>
-      <c r="C224" s="8">
-        <v>1</v>
-      </c>
-      <c r="D224" s="7" t="s">
+      <c r="B224" s="7">
+        <v>1</v>
+      </c>
+      <c r="C224" s="7">
+        <v>1</v>
+      </c>
+      <c r="D224" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E224" t="s">
+      <c r="E224" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A225" s="7" t="s">
+      <c r="A225" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B225" s="8">
-        <v>1</v>
-      </c>
-      <c r="C225" s="8">
+      <c r="B225" s="7">
+        <v>1</v>
+      </c>
+      <c r="C225" s="7">
         <v>2</v>
       </c>
-      <c r="D225" s="7" t="s">
+      <c r="D225" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E225" t="s">
+      <c r="E225" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A226" s="7" t="s">
+      <c r="A226" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B226" s="8">
-        <v>1</v>
-      </c>
-      <c r="C226" s="8">
-        <v>1</v>
-      </c>
-      <c r="D226" s="7" t="s">
+      <c r="B226" s="7">
+        <v>1</v>
+      </c>
+      <c r="C226" s="7">
+        <v>1</v>
+      </c>
+      <c r="D226" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E226" t="s">
+      <c r="E226" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A227" s="7" t="s">
+      <c r="A227" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B227" s="8">
-        <v>1</v>
-      </c>
-      <c r="C227" s="8">
-        <v>3</v>
-      </c>
-      <c r="D227" s="7" t="s">
+      <c r="B227" s="7">
+        <v>1</v>
+      </c>
+      <c r="C227" s="7">
+        <v>3</v>
+      </c>
+      <c r="D227" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E227" t="s">
+      <c r="E227" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A228" s="7" t="s">
+      <c r="A228" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B228" s="8">
-        <v>1</v>
-      </c>
-      <c r="C228" s="8">
-        <v>1</v>
-      </c>
-      <c r="D228" s="7" t="s">
+      <c r="B228" s="7">
+        <v>1</v>
+      </c>
+      <c r="C228" s="7">
+        <v>1</v>
+      </c>
+      <c r="D228" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E228" t="s">
+      <c r="E228" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A229" s="7" t="s">
+      <c r="A229" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B229" s="8">
+      <c r="B229" s="7">
         <v>2</v>
       </c>
-      <c r="C229" s="8">
-        <v>1</v>
-      </c>
-      <c r="D229" s="7" t="s">
+      <c r="C229" s="7">
+        <v>1</v>
+      </c>
+      <c r="D229" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E229" t="s">
+      <c r="E229" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A230" s="7" t="s">
+      <c r="A230" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B230" s="8">
-        <v>1</v>
-      </c>
-      <c r="C230" s="8">
+      <c r="B230" s="7">
+        <v>1</v>
+      </c>
+      <c r="C230" s="7">
         <v>2</v>
       </c>
-      <c r="D230" s="7" t="s">
+      <c r="D230" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E230" t="s">
+      <c r="E230" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A231" s="7" t="s">
+      <c r="A231" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B231" s="8">
-        <v>9</v>
-      </c>
-      <c r="C231" s="8">
-        <v>1</v>
-      </c>
-      <c r="D231" s="7" t="s">
+      <c r="B231" s="7">
+        <v>9</v>
+      </c>
+      <c r="C231" s="7">
+        <v>1</v>
+      </c>
+      <c r="D231" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E231" t="s">
+      <c r="E231" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A232" s="7" t="s">
+      <c r="A232" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B232" s="8">
-        <v>9</v>
-      </c>
-      <c r="C232" s="8">
-        <v>1</v>
-      </c>
-      <c r="D232" s="7" t="s">
+      <c r="B232" s="7">
+        <v>9</v>
+      </c>
+      <c r="C232" s="7">
+        <v>1</v>
+      </c>
+      <c r="D232" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E232" t="s">
+      <c r="E232" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A233" s="7" t="s">
+      <c r="A233" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B233" s="8">
-        <v>9</v>
-      </c>
-      <c r="C233" s="8">
-        <v>1</v>
-      </c>
-      <c r="D233" s="7" t="s">
+      <c r="B233" s="7">
+        <v>9</v>
+      </c>
+      <c r="C233" s="7">
+        <v>1</v>
+      </c>
+      <c r="D233" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E233" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A234" s="7" t="s">
+      <c r="A234" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B234" s="8">
-        <v>9</v>
-      </c>
-      <c r="C234" s="8">
-        <v>1</v>
-      </c>
-      <c r="D234" s="7" t="s">
+      <c r="B234" s="7">
+        <v>9</v>
+      </c>
+      <c r="C234" s="7">
+        <v>1</v>
+      </c>
+      <c r="D234" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E234" t="s">
+      <c r="E234" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A235" s="7" t="s">
+      <c r="A235" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B235" s="8">
-        <v>1</v>
-      </c>
-      <c r="C235" s="8">
-        <v>1</v>
-      </c>
-      <c r="D235" s="7" t="s">
+      <c r="B235" s="7">
+        <v>1</v>
+      </c>
+      <c r="C235" s="7">
+        <v>1</v>
+      </c>
+      <c r="D235" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E235" t="s">
+      <c r="E235" s="8" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>